<commit_message>
Commited changes for Coursera P4E
</commit_message>
<xml_diff>
--- a/Learning-Path/restart_Code_Flow.xlsx
+++ b/Learning-Path/restart_Code_Flow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Restart\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Restart\My Drive\restartmode\Learning-Path\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AEB18E-89D7-41C1-A3E6-7DA2381E17C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DCAB42-DF67-4146-BAA2-E2DD5AC36809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2C407D1D-D7D3-4FAF-B87B-0CBF650F3E4E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Sr</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>Study Designs in Epidemiology</t>
+  </si>
+  <si>
+    <t>Data Science in Stratified Healthcare and Precision Medicine</t>
+  </si>
+  <si>
+    <t>https://www.coursera.org/learn/datascimed</t>
   </si>
 </sst>
 </file>
@@ -781,7 +787,9 @@
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
+      <c r="B17" s="7">
+        <v>13</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
@@ -815,7 +823,7 @@
   <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -935,8 +943,12 @@
       <c r="B12" s="7">
         <v>8</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -980,6 +992,7 @@
     <hyperlink ref="D9" r:id="rId5" xr:uid="{9634A41E-9A94-451D-92C9-3A4358D61E0E}"/>
     <hyperlink ref="D10" r:id="rId6" xr:uid="{509159F4-9C18-4F9D-8DE0-90784D1BDA4F}"/>
     <hyperlink ref="D11" r:id="rId7" xr:uid="{2B936C3F-9C66-4B40-9026-9FA8D231A6AD}"/>
+    <hyperlink ref="D12" r:id="rId8" xr:uid="{36B3E8AC-E7EB-4645-9CD5-6DB614E33672}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Python for Everybody -- Specialization Completed
</commit_message>
<xml_diff>
--- a/Learning-Path/restart_Code_Flow.xlsx
+++ b/Learning-Path/restart_Code_Flow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Restart\My Drive\restartmode\Learning-Path\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DCAB42-DF67-4146-BAA2-E2DD5AC36809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303303E8-66AE-4530-8BD3-66C943091628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2C407D1D-D7D3-4FAF-B87B-0CBF650F3E4E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2C407D1D-D7D3-4FAF-B87B-0CBF650F3E4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Core-Courses" sheetId="1" r:id="rId1"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C74EDC3-5049-4E39-81C0-BA5E096B111F}">
   <dimension ref="B2:E17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -822,7 +822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D500852-F8C5-4FA7-B4B2-922A4785DA66}">
   <dimension ref="B2:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ML Specialization Final Checkin
</commit_message>
<xml_diff>
--- a/Learning-Path/restart_Code_Flow.xlsx
+++ b/Learning-Path/restart_Code_Flow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Restart\My Drive\restartmode\Learning-Path\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6A8D68-22E9-4E15-A5CB-B0CECC2FBD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43BE016-6F78-4C5D-8062-64406E0196D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2C407D1D-D7D3-4FAF-B87B-0CBF650F3E4E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
   <si>
     <t>Sr</t>
   </si>
@@ -665,7 +665,7 @@
   <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B5" sqref="B5:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -700,6 +700,7 @@
     </row>
     <row r="5" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
+        <f>ROW()-4</f>
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -714,6 +715,7 @@
     </row>
     <row r="6" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
+        <f t="shared" ref="B6:B18" si="0">ROW()-4</f>
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -728,6 +730,7 @@
     </row>
     <row r="7" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -736,10 +739,13 @@
       <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -752,30 +758,33 @@
     </row>
     <row r="9" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -788,6 +797,7 @@
     </row>
     <row r="12" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -800,6 +810,7 @@
     </row>
     <row r="13" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -812,6 +823,7 @@
     </row>
     <row r="14" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -824,6 +836,7 @@
     </row>
     <row r="15" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -836,6 +849,7 @@
     </row>
     <row r="16" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -848,6 +862,7 @@
     </row>
     <row r="17" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -860,6 +875,7 @@
     </row>
     <row r="18" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -875,16 +891,16 @@
     <hyperlink ref="D5" r:id="rId1" xr:uid="{1D83BBEE-5188-4023-A85F-6449C695F337}"/>
     <hyperlink ref="D6" r:id="rId2" xr:uid="{509330C1-B362-4155-BE7C-A99742D648D2}"/>
     <hyperlink ref="D7" r:id="rId3" xr:uid="{A2CA7D09-F434-4370-BD29-E88D4923F8B1}"/>
-    <hyperlink ref="D9" r:id="rId4" xr:uid="{C1EFC085-A03F-4B10-8F1D-99B0B2A1770E}"/>
-    <hyperlink ref="D10" r:id="rId5" xr:uid="{DB79DDB6-5CC4-4D7A-8B96-03A336C4EC28}"/>
-    <hyperlink ref="D13" r:id="rId6" xr:uid="{B755ABF8-B3ED-4D79-B46C-C072266A6BA0}"/>
-    <hyperlink ref="D11" r:id="rId7" xr:uid="{AB340253-54CD-4342-93D8-A7B98559539C}"/>
-    <hyperlink ref="D8" r:id="rId8" xr:uid="{88B1CF13-73A2-426F-9F77-514F6D1C5E13}"/>
-    <hyperlink ref="D14" r:id="rId9" xr:uid="{EC3010E4-99AF-49B2-86AE-201BEA7BD9FC}"/>
-    <hyperlink ref="D15" r:id="rId10" xr:uid="{8165E169-66B8-46E4-9AA0-322D10B70588}"/>
-    <hyperlink ref="D17" r:id="rId11" xr:uid="{48707E3C-B328-4307-8AFA-B746A7A42DEC}"/>
-    <hyperlink ref="D18" r:id="rId12" xr:uid="{8BF13F55-4823-47ED-8CDD-EDD9721DC70E}"/>
-    <hyperlink ref="D16" r:id="rId13" xr:uid="{CA5FCD57-CEED-4610-8817-37071388100A}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{DB79DDB6-5CC4-4D7A-8B96-03A336C4EC28}"/>
+    <hyperlink ref="D13" r:id="rId5" xr:uid="{B755ABF8-B3ED-4D79-B46C-C072266A6BA0}"/>
+    <hyperlink ref="D11" r:id="rId6" xr:uid="{AB340253-54CD-4342-93D8-A7B98559539C}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{88B1CF13-73A2-426F-9F77-514F6D1C5E13}"/>
+    <hyperlink ref="D14" r:id="rId8" xr:uid="{EC3010E4-99AF-49B2-86AE-201BEA7BD9FC}"/>
+    <hyperlink ref="D15" r:id="rId9" xr:uid="{8165E169-66B8-46E4-9AA0-322D10B70588}"/>
+    <hyperlink ref="D17" r:id="rId10" xr:uid="{48707E3C-B328-4307-8AFA-B746A7A42DEC}"/>
+    <hyperlink ref="D18" r:id="rId11" xr:uid="{8BF13F55-4823-47ED-8CDD-EDD9721DC70E}"/>
+    <hyperlink ref="D16" r:id="rId12" xr:uid="{CA5FCD57-CEED-4610-8817-37071388100A}"/>
+    <hyperlink ref="D10" r:id="rId13" xr:uid="{C1EFC085-A03F-4B10-8F1D-99B0B2A1770E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId14"/>

</xml_diff>